<commit_message>
implementation du lecteur de metadonnée
</commit_message>
<xml_diff>
--- a/web/upload/private/test.xlsx
+++ b/web/upload/private/test.xlsx
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>928b44677c5a5b6f5d068d2637c597ac.jpeg</t>
   </si>
@@ -119,9 +119,6 @@
     <t>3803e187888f75f44ac6347c4a1a1ebc.jpeg</t>
   </si>
   <si>
-    <t>102c3002154e7899e64c467bb301f533.jpg</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -264,6 +261,18 @@
   </si>
   <si>
     <t>http://www.vimeo.com/25698458</t>
+  </si>
+  <si>
+    <t>102c3002154e7899e64c467bb301f533.jpeg</t>
+  </si>
+  <si>
+    <t>WINDECK</t>
+  </si>
+  <si>
+    <t>Un (ou une) synopsis est un écrit décrivant la totalité ou un aperçu d'une œuvre ou d'une science. Le terme est essentiellement connu pour son usage ...</t>
+  </si>
+  <si>
+    <t>&lt;span style="color:#ff0000"&gt;ALLO PREZI&lt;/span&gt;</t>
   </si>
 </sst>
 </file>
@@ -370,9 +379,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -386,7 +392,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,45 +405,89 @@
     <dxf>
       <font>
         <b val="0"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -768,61 +821,15 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -867,6 +874,12 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -902,29 +915,29 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="E1:E5" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau9" displayName="Tableau9" ref="E1:E5" totalsRowShown="0" dataDxfId="31">
   <autoFilter ref="E1:E5"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="Mention" dataDxfId="4"/>
+    <tableColumn id="1" name="Mention" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="A1:AB4" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau8" displayName="Tableau8" ref="A1:AB4" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:AB4"/>
   <tableColumns count="28">
-    <tableColumn id="1" name="Name" dataDxfId="29"/>
-    <tableColumn id="2" name="Category" dataDxfId="28"/>
-    <tableColumn id="5" name="EpisodeNbr" dataDxfId="5"/>
-    <tableColumn id="6" name="Duration" dataDxfId="2"/>
-    <tableColumn id="7" name="Mention" dataDxfId="0"/>
-    <tableColumn id="11" name="Trailer" dataDxfId="1"/>
-    <tableColumn id="10" name="Episode1" dataDxfId="27"/>
-    <tableColumn id="9" name="Episode2" dataDxfId="26"/>
-    <tableColumn id="8" name="Episode3" dataDxfId="25"/>
-    <tableColumn id="15" name="Synopsis" dataDxfId="24"/>
+    <tableColumn id="1" name="Name" dataDxfId="27"/>
+    <tableColumn id="2" name="Category" dataDxfId="26"/>
+    <tableColumn id="5" name="EpisodeNbr" dataDxfId="25"/>
+    <tableColumn id="6" name="Duration" dataDxfId="24"/>
+    <tableColumn id="7" name="Mention" dataDxfId="5"/>
+    <tableColumn id="11" name="Trailer" dataDxfId="4"/>
+    <tableColumn id="10" name="Episode1" dataDxfId="3"/>
+    <tableColumn id="9" name="Episode2" dataDxfId="2"/>
+    <tableColumn id="8" name="Episode3" dataDxfId="1"/>
+    <tableColumn id="15" name="Synopsis" dataDxfId="0"/>
     <tableColumn id="16" name="Tagline" dataDxfId="23"/>
     <tableColumn id="17" name="Logline" dataDxfId="22"/>
     <tableColumn id="18" name="Rewards" dataDxfId="21"/>
@@ -1238,7 +1251,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1249,81 +1262,81 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1340,8 +1353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1364,113 +1377,121 @@
   <sheetData>
     <row r="1" spans="1:28" s="10" customFormat="1" ht="28.5" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="W1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="AB1" s="13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="25.5" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="16">
+        <v>48</v>
+      </c>
+      <c r="C2" s="15">
         <v>10</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>40</v>
+      <c r="D2" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="F2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>55</v>
+      </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -1483,16 +1504,16 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="X2" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Y2" s="11" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="Z2" s="11" t="s">
         <v>2</v>
@@ -1500,19 +1521,37 @@
       <c r="AA2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="AB2" s="14"/>
+      <c r="AB2" s="13"/>
     </row>
-    <row r="3" spans="1:28">
-      <c r="A3" s="4"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+    <row r="3" spans="1:28" ht="25.5" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="15">
+        <v>45</v>
+      </c>
+      <c r="D3" s="14">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="17"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -1525,13 +1564,13 @@
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y3" s="11" t="s">
         <v>0</v>
@@ -1542,19 +1581,37 @@
       <c r="AA3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="AB3" s="14"/>
+      <c r="AB3" s="13"/>
     </row>
-    <row r="4" spans="1:28">
-      <c r="A4" s="4"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+    <row r="4" spans="1:28" ht="25.5" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="15">
+        <v>25</v>
+      </c>
+      <c r="D4" s="14">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="17"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -1567,18 +1624,18 @@
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="14"/>
+        <v>32</v>
+      </c>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="3">

</xml_diff>